<commit_message>
Mail v1.2, notule ceo v2.0
+- Mail
+- notule ceo
</commit_message>
<xml_diff>
--- a/documentatie/notulen/interview/notule_interview_ceo.xlsx
+++ b/documentatie/notulen/interview/notule_interview_ceo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef\Documents\GitKraken\Barroc-IT-Groep-2\documentation\notulen\interview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef\Documents\GitKraken\Barroc-IT-Groep-2\documentatie\notulen\interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>Onderwerp</t>
   </si>
@@ -114,16 +114,10 @@
     <t>9 Tijdsduur</t>
   </si>
   <si>
-    <t>10 Updates project</t>
-  </si>
-  <si>
     <t>4 Functies</t>
   </si>
   <si>
     <t>Slecht, geven nauwelijk informatie aan elkaar door.</t>
-  </si>
-  <si>
-    <t>13 Sluiting</t>
   </si>
   <si>
     <t>1 Openen</t>
@@ -310,10 +304,58 @@
     <t>Afdelingen mogen elkaar informatie niet aanpassen, alleen de informatie die voor de afdelingen nodig zijn mogen ze aanpassen. De informatie mag wel doorgegeven worden.  Sommige informatie hoefen niet beschikbaar te zijn voor andere afdelingen.</t>
   </si>
   <si>
-    <t>12 Terugoppeling interview en offerte</t>
+    <t>10 Taal applicatie</t>
   </si>
   <si>
-    <t>13 Rondvraag</t>
+    <t>De taal van de applicatie</t>
+  </si>
+  <si>
+    <t>De heer van Bueren</t>
+  </si>
+  <si>
+    <t>11 Helpfunctie</t>
+  </si>
+  <si>
+    <t>De helpfunctie van de applicatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wij willen graag voor onze collega's een helpfunctie zowel in het Nederlands als in het Engels. De helpfunctie is bedoeld voor collega's die eigenlijk info willen wat iets doet.</t>
+  </si>
+  <si>
+    <t>12 Plan van Aanpak</t>
+  </si>
+  <si>
+    <t>Aangezien de collega's van heer Vorselaars Engelstalig zijn willen we de applicatie in het Engels.</t>
+  </si>
+  <si>
+    <t>Het plan hoe de opdrachtnemers alles gaan aanpakken</t>
+  </si>
+  <si>
+    <t>Mijn collega's en ik verwachten dat de plan van aanpak in het Engels wordt geschreven omdat we Engelse collega's hebben.</t>
+  </si>
+  <si>
+    <t>Voor de ontwikkeling van de applicatie</t>
+  </si>
+  <si>
+    <t>14 Updates project</t>
+  </si>
+  <si>
+    <t>16 Rondvraag</t>
+  </si>
+  <si>
+    <t>17 Sluiting</t>
+  </si>
+  <si>
+    <t>13 Opdracht vaststellen</t>
+  </si>
+  <si>
+    <t>De opdracht van de opdrachtgever vaststellen</t>
+  </si>
+  <si>
+    <t>Kort samengevat, de heer van Bueren wilt een applicatie met daarin een opslagplek voor alle klanten data. Daarnaast moet de afdeling Sales facturen kunnen maken. Dit gaat ervoor zorgen dat de afdelingen geen fouten meer maken waardoor ze sneller en beter gaan werken.</t>
+  </si>
+  <si>
+    <t>15 Terugkoppeling interview en offerte</t>
   </si>
 </sst>
 </file>
@@ -469,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -562,15 +604,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -927,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q14022"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +975,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="2"/>
@@ -966,7 +999,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="23"/>
@@ -989,7 +1022,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="23"/>
@@ -1012,7 +1045,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="23"/>
@@ -1032,10 +1065,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="23"/>
@@ -1084,10 +1117,10 @@
     </row>
     <row r="7" spans="1:17" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>9</v>
@@ -1113,13 +1146,13 @@
     </row>
     <row r="8" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>12</v>
@@ -1145,7 +1178,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>13</v>
@@ -1154,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -1171,13 +1204,13 @@
     </row>
     <row r="10" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>16</v>
@@ -1203,10 +1236,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>11</v>
@@ -1220,10 +1253,10 @@
         <v>18</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>11</v>
@@ -1237,10 +1270,10 @@
         <v>19</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>11</v>
@@ -1254,7 +1287,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>15</v>
@@ -1263,7 +1296,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="51" x14ac:dyDescent="0.25">
@@ -1271,10 +1304,10 @@
         <v>20</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>11</v>
@@ -1283,101 +1316,141 @@
         <v>43036</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="153" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>21</v>
+    <row r="16" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>56</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>29</v>
+      <c r="B16" s="21" t="s">
+        <v>57</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:5" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>30</v>
+      <c r="E17" s="27" t="s">
+        <v>52</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>43</v>
+    </row>
+    <row r="18" spans="1:5" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>62</v>
       </c>
-      <c r="D17" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>31</v>
+      <c r="B18" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>24</v>
+    <row r="19" spans="1:5" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>9</v>
+      <c r="C19" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E19" s="27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
+    <row r="20" spans="1:5" ht="153" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="51" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
+      <c r="A23" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>

</xml_diff>